<commit_message>
major update channel renaming and refactoring
</commit_message>
<xml_diff>
--- a/icn_bids/templates/CHARITE_CHANNEL_NAMING.xlsx
+++ b/icn_bids/templates/CHARITE_CHANNEL_NAMING.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://charitede.sharepoint.com/sites/AGBewegungsstrungen-LFP-Labor/Shared Documents/LFP-Labor/FileAndChannelNaming/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonathan\Documents\CODE\icn\icn_bids\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="364" documentId="8_{CFAF6246-B4F7-4696-A1D5-C589A02A1D1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{33FAFCB5-EA64-4007-9F57-DFA55DE7E83C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5CF921-F6B5-4CFD-9A67-CFF38D808CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="690" xr2:uid="{89569B8A-D8E6-4033-88F6-D23FA03DC854}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="690" xr2:uid="{89569B8A-D8E6-4033-88F6-D23FA03DC854}"/>
   </bookViews>
   <sheets>
     <sheet name="Boston - TMSi" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1483" uniqueCount="155">
   <si>
     <t>Channel naming schemes in the Interventional and Cognitive Neuromodulation group and the CRCNS iDBS collaboration</t>
   </si>
@@ -491,6 +491,18 @@
   </si>
   <si>
     <t>R/L</t>
+  </si>
+  <si>
+    <t>CZ_</t>
+  </si>
+  <si>
+    <t>FZ</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>FZ_</t>
   </si>
 </sst>
 </file>
@@ -830,7 +842,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -846,7 +858,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1144,30 +1156,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09D03CD8-37D9-4F50-B3CF-F78391FE3950}">
   <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.26953125" customWidth="1"/>
-    <col min="4" max="4" width="6.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" customWidth="1"/>
-    <col min="8" max="9" width="16.54296875" customWidth="1"/>
-    <col min="10" max="10" width="27.7265625" customWidth="1"/>
-    <col min="11" max="11" width="26.81640625" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" customWidth="1"/>
-    <col min="14" max="14" width="18.1796875" customWidth="1"/>
-    <col min="15" max="16" width="23.7265625" customWidth="1"/>
-    <col min="17" max="17" width="58.7265625" customWidth="1"/>
-    <col min="18" max="18" width="29.1796875" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="15" max="16" width="23.7109375" customWidth="1"/>
+    <col min="17" max="17" width="58.7109375" customWidth="1"/>
+    <col min="18" max="18" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1188,7 +1200,7 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1207,7 +1219,7 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1228,7 +1240,7 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1251,7 +1263,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1274,7 +1286,7 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1292,7 +1304,7 @@
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
     </row>
-    <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
@@ -1343,7 +1355,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>21</v>
       </c>
@@ -1397,7 +1409,7 @@
       </c>
       <c r="T8" s="6"/>
     </row>
-    <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>30</v>
       </c>
@@ -1447,7 +1459,7 @@
       </c>
       <c r="S9" s="9"/>
     </row>
-    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>34</v>
       </c>
@@ -1497,7 +1509,7 @@
       </c>
       <c r="S10" s="9"/>
     </row>
-    <row r="11" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>38</v>
       </c>
@@ -1550,7 +1562,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>44</v>
       </c>
@@ -1599,7 +1611,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
@@ -1644,7 +1656,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>50</v>
       </c>
@@ -1697,7 +1709,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>55</v>
       </c>
@@ -1744,7 +1756,7 @@
       </c>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>58</v>
       </c>
@@ -1797,7 +1809,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>62</v>
       </c>
@@ -1847,7 +1859,7 @@
       </c>
       <c r="T17" s="7"/>
     </row>
-    <row r="18" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>64</v>
       </c>
@@ -1893,7 +1905,7 @@
       </c>
       <c r="T18" s="6"/>
     </row>
-    <row r="19" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>66</v>
       </c>
@@ -1938,7 +1950,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>68</v>
       </c>
@@ -1984,7 +1996,7 @@
       </c>
       <c r="T20" s="7"/>
     </row>
-    <row r="21" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>70</v>
       </c>
@@ -2039,7 +2051,7 @@
       <c r="S21" s="8"/>
       <c r="T21" s="6"/>
     </row>
-    <row r="22" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>73</v>
       </c>
@@ -2087,7 +2099,7 @@
       <c r="Q22" s="23"/>
       <c r="S22" s="9"/>
     </row>
-    <row r="23" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>74</v>
       </c>
@@ -2141,7 +2153,7 @@
       </c>
       <c r="S23" s="7"/>
     </row>
-    <row r="24" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>80</v>
       </c>
@@ -2173,7 +2185,7 @@
       <c r="Q24" s="1"/>
       <c r="S24" s="7"/>
     </row>
-    <row r="25" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="38" t="s">
         <v>82</v>
       </c>
@@ -2205,7 +2217,7 @@
       <c r="Q25" s="1"/>
       <c r="S25" s="7"/>
     </row>
-    <row r="26" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="38" t="s">
         <v>83</v>
       </c>
@@ -2237,7 +2249,7 @@
       <c r="Q26" s="1"/>
       <c r="S26" s="7"/>
     </row>
-    <row r="27" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="38" t="s">
         <v>84</v>
       </c>
@@ -2270,7 +2282,7 @@
       <c r="S27" s="7"/>
       <c r="T27" s="7"/>
     </row>
-    <row r="28" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="38" t="s">
         <v>85</v>
       </c>
@@ -2303,7 +2315,7 @@
       <c r="S28" s="7"/>
       <c r="T28" s="6"/>
     </row>
-    <row r="29" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="38" t="s">
         <v>86</v>
       </c>
@@ -2335,7 +2347,7 @@
       <c r="Q29" s="1"/>
       <c r="S29" s="7"/>
     </row>
-    <row r="30" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="38" t="s">
         <v>87</v>
       </c>
@@ -2368,7 +2380,7 @@
       <c r="S30" s="7"/>
       <c r="T30" s="7"/>
     </row>
-    <row r="31" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="39" t="s">
         <v>88</v>
       </c>
@@ -2401,7 +2413,7 @@
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
     </row>
-    <row r="32" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>89</v>
       </c>
@@ -2446,7 +2458,7 @@
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
     </row>
-    <row r="33" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>93</v>
       </c>
@@ -2489,7 +2501,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>94</v>
       </c>
@@ -2532,7 +2544,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>95</v>
       </c>
@@ -2575,7 +2587,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
         <v>96</v>
       </c>
@@ -2618,7 +2630,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>97</v>
       </c>
@@ -2661,7 +2673,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
         <v>98</v>
       </c>
@@ -2678,10 +2690,10 @@
         <v>1</v>
       </c>
       <c r="F38" s="22" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
       <c r="G38" s="22" t="s">
-        <v>101</v>
+        <v>153</v>
       </c>
       <c r="H38" s="22" t="s">
         <v>102</v>
@@ -2691,11 +2703,11 @@
       </c>
       <c r="J38" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>EEGC1Cz_T</v>
+        <v>EEGC1CZ_T</v>
       </c>
       <c r="K38" s="35" t="str">
         <f>CONCATENATE(C38,"_",G38,"_",I38)</f>
-        <v>EEG_Cz_TM</v>
+        <v>EEG_CZ_TM</v>
       </c>
       <c r="L38" s="1"/>
       <c r="M38" s="1"/>
@@ -2704,7 +2716,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>104</v>
       </c>
@@ -2721,10 +2733,10 @@
         <v>2</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>105</v>
+        <v>154</v>
       </c>
       <c r="G39" s="22" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="H39" s="22" t="s">
         <v>102</v>
@@ -2734,11 +2746,11 @@
       </c>
       <c r="J39" s="32" t="str">
         <f t="shared" si="0"/>
-        <v>EEGC2Fz_T</v>
+        <v>EEGC2FZ_T</v>
       </c>
       <c r="K39" s="35" t="str">
         <f>CONCATENATE(C39,"_",G39,"_",I39)</f>
-        <v>EEG_Fz_TM</v>
+        <v>EEG_FZ_TM</v>
       </c>
       <c r="L39" s="1"/>
       <c r="M39" s="1"/>
@@ -2747,7 +2759,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>107</v>
       </c>
@@ -2789,7 +2801,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30"/>
       <c r="B41" s="19" t="s">
         <v>71</v>
@@ -2829,7 +2841,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="25"/>
       <c r="B42" s="22" t="s">
         <v>71</v>
@@ -2869,7 +2881,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="30" t="s">
         <v>113</v>
       </c>
@@ -2911,7 +2923,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
       <c r="B44" s="19" t="s">
         <v>71</v>
@@ -2951,7 +2963,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="25"/>
       <c r="B45" s="22" t="s">
         <v>71</v>
@@ -2991,7 +3003,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
         <v>114</v>
       </c>
@@ -3034,7 +3046,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30" t="s">
         <v>118</v>
       </c>
@@ -3076,7 +3088,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="22" t="s">
         <v>60</v>
@@ -3134,26 +3146,26 @@
       <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="6" width="10.81640625" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" customWidth="1"/>
-    <col min="8" max="8" width="18.54296875" customWidth="1"/>
-    <col min="9" max="9" width="15.54296875" customWidth="1"/>
-    <col min="10" max="10" width="27.453125" customWidth="1"/>
-    <col min="11" max="11" width="27.54296875" customWidth="1"/>
-    <col min="13" max="13" width="17.7265625" customWidth="1"/>
-    <col min="14" max="14" width="16.81640625" customWidth="1"/>
-    <col min="15" max="15" width="20.453125" customWidth="1"/>
-    <col min="16" max="16" width="29.1796875" customWidth="1"/>
+    <col min="5" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="27.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.5703125" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="16.85546875" customWidth="1"/>
+    <col min="15" max="15" width="20.42578125" customWidth="1"/>
+    <col min="16" max="16" width="29.140625" customWidth="1"/>
     <col min="17" max="17" width="59" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3172,7 +3184,7 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -3189,7 +3201,7 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -3208,7 +3220,7 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3229,7 +3241,7 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -3250,7 +3262,7 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" s="1"/>
@@ -3266,7 +3278,7 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
@@ -3317,7 +3329,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>21</v>
       </c>
@@ -3371,7 +3383,7 @@
       </c>
       <c r="R8" s="6"/>
     </row>
-    <row r="9" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>30</v>
       </c>
@@ -3420,7 +3432,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>34</v>
       </c>
@@ -3469,7 +3481,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>38</v>
       </c>
@@ -3522,7 +3534,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>44</v>
       </c>
@@ -3571,7 +3583,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
@@ -3616,7 +3628,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>50</v>
       </c>
@@ -3669,7 +3681,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>55</v>
       </c>
@@ -3716,7 +3728,7 @@
       </c>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>58</v>
       </c>
@@ -3769,7 +3781,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>62</v>
       </c>
@@ -3819,7 +3831,7 @@
       </c>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>64</v>
       </c>
@@ -3865,7 +3877,7 @@
       </c>
       <c r="R18" s="6"/>
     </row>
-    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>66</v>
       </c>
@@ -3910,7 +3922,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>68</v>
       </c>
@@ -3956,7 +3968,7 @@
       </c>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>70</v>
       </c>
@@ -4010,7 +4022,7 @@
       </c>
       <c r="R21" s="6"/>
     </row>
-    <row r="22" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>73</v>
       </c>
@@ -4057,7 +4069,7 @@
       </c>
       <c r="Q22" s="23"/>
     </row>
-    <row r="23" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>74</v>
       </c>
@@ -4110,7 +4122,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>80</v>
       </c>
@@ -4140,7 +4152,7 @@
       <c r="O24" s="1"/>
       <c r="Q24" s="7"/>
     </row>
-    <row r="25" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="38" t="s">
         <v>82</v>
       </c>
@@ -4170,7 +4182,7 @@
       <c r="O25" s="1"/>
       <c r="Q25" s="7"/>
     </row>
-    <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="38" t="s">
         <v>83</v>
       </c>
@@ -4200,7 +4212,7 @@
       <c r="O26" s="1"/>
       <c r="Q26" s="7"/>
     </row>
-    <row r="27" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="38" t="s">
         <v>84</v>
       </c>
@@ -4231,7 +4243,7 @@
       <c r="Q27" s="7"/>
       <c r="R27" s="7"/>
     </row>
-    <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="38" t="s">
         <v>85</v>
       </c>
@@ -4262,7 +4274,7 @@
       <c r="Q28" s="7"/>
       <c r="R28" s="6"/>
     </row>
-    <row r="29" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="38" t="s">
         <v>86</v>
       </c>
@@ -4292,7 +4304,7 @@
       <c r="O29" s="1"/>
       <c r="Q29" s="7"/>
     </row>
-    <row r="30" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="38" t="s">
         <v>87</v>
       </c>
@@ -4323,7 +4335,7 @@
       <c r="Q30" s="7"/>
       <c r="R30" s="7"/>
     </row>
-    <row r="31" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="39" t="s">
         <v>88</v>
       </c>
@@ -4354,7 +4366,7 @@
       <c r="Q31" s="7"/>
       <c r="R31" s="7"/>
     </row>
-    <row r="32" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>89</v>
       </c>
@@ -4397,7 +4409,7 @@
       <c r="Q32" s="7"/>
       <c r="R32" s="7"/>
     </row>
-    <row r="33" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>93</v>
       </c>
@@ -4438,7 +4450,7 @@
       <c r="N33" s="1"/>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>94</v>
       </c>
@@ -4479,7 +4491,7 @@
       <c r="N34" s="1"/>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="27" t="s">
         <v>95</v>
       </c>
@@ -4520,7 +4532,7 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
         <v>96</v>
       </c>
@@ -4561,7 +4573,7 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>97</v>
       </c>
@@ -4602,7 +4614,7 @@
       <c r="N37" s="1"/>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
         <v>98</v>
       </c>
@@ -4643,7 +4655,7 @@
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>104</v>
       </c>
@@ -4684,7 +4696,7 @@
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>107</v>
       </c>
@@ -4724,7 +4736,7 @@
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
     </row>
-    <row r="41" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30"/>
       <c r="B41" s="19" t="s">
         <v>71</v>
@@ -4762,7 +4774,7 @@
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
     </row>
-    <row r="42" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="25"/>
       <c r="B42" s="22" t="s">
         <v>71</v>
@@ -4800,7 +4812,7 @@
       <c r="N42" s="1"/>
       <c r="O42" s="1"/>
     </row>
-    <row r="43" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="30" t="s">
         <v>113</v>
       </c>
@@ -4840,7 +4852,7 @@
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
     </row>
-    <row r="44" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
       <c r="B44" s="19" t="s">
         <v>71</v>
@@ -4878,7 +4890,7 @@
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
     </row>
-    <row r="45" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="25"/>
       <c r="B45" s="22" t="s">
         <v>71</v>
@@ -4916,7 +4928,7 @@
       <c r="N45" s="1"/>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
         <v>114</v>
       </c>
@@ -4957,7 +4969,7 @@
       <c r="N46" s="1"/>
       <c r="O46" s="1"/>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="30" t="s">
         <v>118</v>
       </c>
@@ -4995,7 +5007,7 @@
       <c r="N47" s="1"/>
       <c r="O47" s="1"/>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="22" t="s">
         <v>60</v>
@@ -5045,27 +5057,27 @@
       <selection activeCell="K38" sqref="K38:K48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="11.1796875" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" customWidth="1"/>
-    <col min="9" max="9" width="16.7265625" customWidth="1"/>
-    <col min="10" max="10" width="27.54296875" customWidth="1"/>
-    <col min="11" max="11" width="35.1796875" customWidth="1"/>
-    <col min="13" max="13" width="16.54296875" customWidth="1"/>
-    <col min="14" max="14" width="16.453125" customWidth="1"/>
-    <col min="15" max="15" width="18.7265625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" customWidth="1"/>
+    <col min="11" max="11" width="35.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
     <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="24.54296875" customWidth="1"/>
+    <col min="17" max="17" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5076,7 +5088,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -5085,7 +5097,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -5096,7 +5108,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -5111,7 +5123,7 @@
       <c r="H4" s="41"/>
       <c r="I4" s="41"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -5124,7 +5136,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -5133,7 +5145,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
@@ -5184,7 +5196,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="33" t="s">
         <v>21</v>
       </c>
@@ -5237,7 +5249,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="27" t="s">
         <v>30</v>
       </c>
@@ -5286,7 +5298,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="30" t="s">
         <v>34</v>
       </c>
@@ -5335,7 +5347,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>38</v>
       </c>
@@ -5388,7 +5400,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>44</v>
       </c>
@@ -5437,7 +5449,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>48</v>
       </c>
@@ -5482,7 +5494,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>50</v>
       </c>
@@ -5535,7 +5547,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>55</v>
       </c>
@@ -5582,7 +5594,7 @@
       </c>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>58</v>
       </c>
@@ -5635,7 +5647,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>62</v>
       </c>
@@ -5684,7 +5696,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>64</v>
       </c>
@@ -5729,7 +5741,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>66</v>
       </c>
@@ -5774,7 +5786,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="15" t="s">
         <v>68</v>
       </c>
@@ -5819,7 +5831,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="15" t="s">
         <v>70</v>
       </c>
@@ -5872,7 +5884,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="15" t="s">
         <v>73</v>
       </c>
@@ -5919,7 +5931,7 @@
       </c>
       <c r="Q22" s="23"/>
     </row>
-    <row r="23" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
         <v>74</v>
       </c>
@@ -5972,7 +5984,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>80</v>
       </c>
@@ -6003,7 +6015,7 @@
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
     </row>
-    <row r="25" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="38" t="s">
         <v>82</v>
       </c>
@@ -6034,7 +6046,7 @@
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
     </row>
-    <row r="26" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="38" t="s">
         <v>83</v>
       </c>
@@ -6065,7 +6077,7 @@
       <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
     </row>
-    <row r="27" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="38" t="s">
         <v>84</v>
       </c>
@@ -6096,7 +6108,7 @@
       <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="38" t="s">
         <v>85</v>
       </c>
@@ -6127,7 +6139,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="38" t="s">
         <v>86</v>
       </c>
@@ -6158,7 +6170,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="38" t="s">
         <v>87</v>
       </c>
@@ -6189,7 +6201,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="39" t="s">
         <v>88</v>
       </c>
@@ -6220,7 +6232,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>89</v>
       </c>
@@ -6251,7 +6263,7 @@
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
     </row>
-    <row r="33" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
         <v>93</v>
       </c>
@@ -6282,7 +6294,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="27" t="s">
         <v>94</v>
       </c>
@@ -6313,7 +6325,7 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
     </row>
-    <row r="35" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="25" t="s">
         <v>95</v>
       </c>
@@ -6344,7 +6356,7 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
     </row>
-    <row r="36" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="25" t="s">
         <v>96</v>
       </c>
@@ -6375,7 +6387,7 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
     </row>
-    <row r="37" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>97</v>
       </c>
@@ -6406,7 +6418,7 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
     </row>
-    <row r="38" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="25" t="s">
         <v>98</v>
       </c>
@@ -6437,7 +6449,7 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
     </row>
-    <row r="39" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="25" t="s">
         <v>104</v>
       </c>
@@ -6468,7 +6480,7 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
     </row>
-    <row r="40" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="15" t="s">
         <v>107</v>
       </c>
@@ -6510,7 +6522,7 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
     </row>
-    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="30"/>
       <c r="B41" s="19" t="s">
         <v>71</v>
@@ -6550,7 +6562,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
     </row>
-    <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="25"/>
       <c r="B42" s="22" t="s">
         <v>71</v>
@@ -6590,7 +6602,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
     </row>
-    <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="30" t="s">
         <v>113</v>
       </c>
@@ -6632,7 +6644,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
     </row>
-    <row r="44" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
       <c r="B44" s="19" t="s">
         <v>71</v>
@@ -6672,7 +6684,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
     </row>
-    <row r="45" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="25"/>
       <c r="B45" s="22" t="s">
         <v>71</v>
@@ -6712,7 +6724,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
     </row>
-    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="27" t="s">
         <v>114</v>
       </c>
@@ -6755,7 +6767,7 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
     </row>
-    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="30" t="s">
         <v>118</v>
       </c>
@@ -6797,7 +6809,7 @@
       <c r="P47" s="1"/>
       <c r="Q47" s="1"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="25"/>
       <c r="B48" s="22" t="s">
         <v>60</v>
@@ -6850,25 +6862,25 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="6" width="13.453125" customWidth="1"/>
-    <col min="7" max="7" width="17.453125" customWidth="1"/>
+    <col min="5" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="30.453125" customWidth="1"/>
-    <col min="10" max="10" width="32.26953125" customWidth="1"/>
-    <col min="12" max="12" width="15.54296875" customWidth="1"/>
-    <col min="13" max="13" width="16.1796875" customWidth="1"/>
-    <col min="14" max="14" width="18.81640625" customWidth="1"/>
-    <col min="15" max="15" width="20.1796875" customWidth="1"/>
-    <col min="16" max="16" width="58.81640625" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" customWidth="1"/>
+    <col min="10" max="10" width="32.28515625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" customWidth="1"/>
+    <col min="16" max="16" width="58.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6886,7 +6898,7 @@
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -6902,7 +6914,7 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -6920,7 +6932,7 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -6940,7 +6952,7 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -6960,7 +6972,7 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
     </row>
-    <row r="6" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" s="1"/>
@@ -6975,7 +6987,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
     </row>
-    <row r="7" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
@@ -7023,7 +7035,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>130</v>
       </c>
@@ -7074,7 +7086,7 @@
       </c>
       <c r="Q8" s="6"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>131</v>
       </c>
@@ -7120,7 +7132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>132</v>
       </c>
@@ -7166,7 +7178,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>133</v>
       </c>
@@ -7216,7 +7228,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>134</v>
       </c>
@@ -7262,7 +7274,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>135</v>
       </c>
@@ -7304,7 +7316,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>136</v>
       </c>
@@ -7354,7 +7366,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>137</v>
       </c>
@@ -7398,7 +7410,7 @@
       </c>
       <c r="P15" s="23"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>138</v>
       </c>
@@ -7448,7 +7460,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>139</v>
       </c>
@@ -7495,7 +7507,7 @@
       </c>
       <c r="Q17" s="7"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>140</v>
       </c>
@@ -7538,7 +7550,7 @@
       </c>
       <c r="Q18" s="6"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>141</v>
       </c>
@@ -7580,7 +7592,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>142</v>
       </c>
@@ -7623,7 +7635,7 @@
       </c>
       <c r="Q20" s="7"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>143</v>
       </c>
@@ -7674,7 +7686,7 @@
       </c>
       <c r="Q21" s="6"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>144</v>
       </c>
@@ -7718,7 +7730,7 @@
       </c>
       <c r="P22" s="23"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>145</v>
       </c>
@@ -7768,7 +7780,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>146</v>
       </c>
@@ -7806,7 +7818,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>148</v>
       </c>
@@ -7844,7 +7856,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>149</v>
       </c>
@@ -7896,27 +7908,27 @@
       <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="10.453125" customWidth="1"/>
-    <col min="3" max="3" width="7.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" customWidth="1"/>
-    <col min="7" max="7" width="16.1796875" customWidth="1"/>
-    <col min="8" max="8" width="16.7265625" customWidth="1"/>
-    <col min="9" max="9" width="28.26953125" customWidth="1"/>
-    <col min="10" max="10" width="27.81640625" customWidth="1"/>
-    <col min="11" max="11" width="19.81640625" customWidth="1"/>
-    <col min="12" max="12" width="15.81640625" customWidth="1"/>
-    <col min="13" max="13" width="17.1796875" customWidth="1"/>
-    <col min="14" max="14" width="20.81640625" customWidth="1"/>
-    <col min="15" max="15" width="19.26953125" customWidth="1"/>
-    <col min="16" max="16" width="42.54296875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" customWidth="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" customWidth="1"/>
+    <col min="16" max="16" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -7931,7 +7943,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -7944,7 +7956,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -7959,7 +7971,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -7976,7 +7988,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -7993,7 +8005,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="D6" s="1"/>
@@ -8005,7 +8017,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>6</v>
       </c>
@@ -8053,7 +8065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>130</v>
       </c>
@@ -8103,7 +8115,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>131</v>
       </c>
@@ -8149,7 +8161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>132</v>
       </c>
@@ -8195,7 +8207,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>133</v>
       </c>
@@ -8245,7 +8257,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>134</v>
       </c>
@@ -8291,7 +8303,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>135</v>
       </c>
@@ -8333,7 +8345,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>136</v>
       </c>
@@ -8383,7 +8395,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>137</v>
       </c>
@@ -8427,7 +8439,7 @@
       </c>
       <c r="P15" s="23"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>138</v>
       </c>
@@ -8477,7 +8489,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>139</v>
       </c>
@@ -8523,7 +8535,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>140</v>
       </c>
@@ -8565,7 +8577,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>141</v>
       </c>
@@ -8607,7 +8619,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="30" t="s">
         <v>142</v>
       </c>
@@ -8649,7 +8661,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>143</v>
       </c>
@@ -8699,7 +8711,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>144</v>
       </c>
@@ -8743,7 +8755,7 @@
       </c>
       <c r="P22" s="23"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>145</v>
       </c>
@@ -8793,7 +8805,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>146</v>
       </c>
@@ -8831,7 +8843,7 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>148</v>
       </c>
@@ -8869,7 +8881,7 @@
       <c r="M25" s="1"/>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>149</v>
       </c>
@@ -8915,21 +8927,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B7A86FA7F3BDCA4697BB6650C7941CF5" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0038c41726a3cbfeea49429cb67666a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e4062f6a-11e6-4d7b-a444-75ffaaa44e33" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a69936769336e44384ab32d8045d793" ns2:_="">
     <xsd:import namespace="e4062f6a-11e6-4d7b-a444-75ffaaa44e33"/>
@@ -9113,11 +9110,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB7DED0E-3063-4CA1-A1D1-C9ECBAE78138}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E91995FF-7E4A-45AB-8304-6F4BC099517B}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e4062f6a-11e6-4d7b-a444-75ffaaa44e33"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9131,5 +9152,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E91995FF-7E4A-45AB-8304-6F4BC099517B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB7DED0E-3063-4CA1-A1D1-C9ECBAE78138}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>